<commit_message>
Added error checking, incomplete
</commit_message>
<xml_diff>
--- a/Statistics/Low Desk/2019/October/LD Week of October 7, 2019.xlsx
+++ b/Statistics/Low Desk/2019/October/LD Week of October 7, 2019.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fordy\Desktop\One Stop GitHub\onestop-excel-processor\Statistics\Low Desk\2019\October\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A8CB61-FE2C-463B-988C-80224E9DC010}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="630" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="6" r:id="rId1"/>
@@ -13,12 +19,20 @@
     <sheet name="Thursday" sheetId="1" r:id="rId4"/>
     <sheet name="Friday" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="12">
   <si>
     <t>Bursar</t>
   </si>
@@ -52,11 +66,14 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>refund info</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,6 +240,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -270,7 +290,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,9 +323,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -338,6 +375,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -513,15 +567,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A1:N85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q3" sqref="Q3:Q5"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +654,9 @@
         <v>8</v>
       </c>
       <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
       <c r="D3" s="8"/>
       <c r="E3" s="7"/>
       <c r="F3" s="8"/>
@@ -611,7 +667,9 @@
       <c r="K3" s="7"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="2"/>
+      <c r="N3" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
@@ -1677,7 +1735,7 @@
       </c>
       <c r="C82" s="11">
         <f t="shared" ref="C82:M82" si="0">SUM(C3:C40)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82" s="11">
         <f t="shared" si="0"/>
@@ -1721,7 +1779,7 @@
       </c>
       <c r="N82" s="11">
         <f>SUM(B82:M82)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
@@ -1848,7 +1906,7 @@
       </c>
       <c r="C85" s="11">
         <f t="shared" ref="C85:N85" si="4">SUM(C82:C84)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D85" s="11">
         <f t="shared" si="4"/>
@@ -1892,7 +1950,7 @@
       </c>
       <c r="N85" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1903,7 +1961,7 @@
     <mergeCell ref="K1:M1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A70" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$Q$3:$Q$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -1912,7 +1970,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -3311,7 +3369,7 @@
     <mergeCell ref="K1:M1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A70" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$Q$3:$Q$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -3320,7 +3378,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -4719,7 +4777,7 @@
     <mergeCell ref="K1:M1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A70" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>$Q$3:$Q$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -4728,7 +4786,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
@@ -6127,7 +6185,7 @@
     <mergeCell ref="K1:M1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A70" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>$Q$3:$Q$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -6136,7 +6194,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -7535,7 +7593,7 @@
     <mergeCell ref="K1:M1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A70" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>$Q$3:$Q$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>